<commit_message>
изменено:      Dockerfile 	изменено:      README.md 	изменено:      data/actual_table.xlsx 	новый файл:    data/instruction.JPG 	изменено:      data/log.log 	изменено:      data/req_archive.xlsx 	изменено:      main_script.py
</commit_message>
<xml_diff>
--- a/data/req_archive.xlsx
+++ b/data/req_archive.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,35 +443,182 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>REQ0717399</t>
+          <t>REQ0782445</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>REQ0715319</t>
+          <t>REQ0782366</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>REQ0714742</t>
+          <t>REQ0782025</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>REQ0714563</t>
+          <t>REQ0781660</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>REQ0714396</t>
+          <t>REQ0781412</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>REQ0781385</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>REQ0780724</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>REQ0780718</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>REQ0780623</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>REQ0777639</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>REQ0770139</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>REQ0767628</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>REQ0767543</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>REQ0767475</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>REQ0767407</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>REQ0767333</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>REQ0767300</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>REQ0767209</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>REQ0767158</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>REQ0759241</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>REQ0759224</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>REQ0759215</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>REQ0759187</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>REQ0759135</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>REQ0758818</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>REQ0753679</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update table load script
</commit_message>
<xml_diff>
--- a/data/req_archive.xlsx
+++ b/data/req_archive.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,180 +443,110 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>REQ0782445</t>
+          <t>REQ0784315</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>REQ0782366</t>
+          <t>REQ0783970</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>REQ0782025</t>
+          <t>REQ0783927</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>REQ0781660</t>
+          <t>REQ0782025</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>REQ0781412</t>
+          <t>REQ0781660</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>REQ0781385</t>
+          <t>REQ0781412</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>REQ0780724</t>
+          <t>REQ0781385</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>REQ0780718</t>
+          <t>REQ0770139</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>REQ0780623</t>
+          <t>REQ0767158</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>REQ0777639</t>
+          <t>REQ0759241</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>REQ0770139</t>
+          <t>REQ0759224</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>REQ0767628</t>
+          <t>REQ0759215</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>REQ0767543</t>
+          <t>REQ0759187</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>REQ0767475</t>
+          <t>REQ0759135</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>REQ0767407</t>
+          <t>REQ0758818</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
-        <is>
-          <t>REQ0767333</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>REQ0767300</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>REQ0767209</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>REQ0767158</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>REQ0759241</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>REQ0759224</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>REQ0759215</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>REQ0759187</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>REQ0759135</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>REQ0758818</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
         <is>
           <t>REQ0753679</t>
         </is>

</xml_diff>